<commit_message>
CIERRE 9 FEB 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/ENTRADAS OBRADOR ENERO 2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/ENTRADAS OBRADOR ENERO 2022.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="96">
   <si>
     <t>FECHA DE PAGO</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>AGROPECUARIA EL TOPETE  247</t>
-  </si>
-  <si>
-    <t>CANALES 49</t>
   </si>
   <si>
     <t>AGROPECUARIA EL TOPETE   250-1</t>
@@ -303,6 +300,18 @@
   </si>
   <si>
     <t>0870 Y.</t>
+  </si>
+  <si>
+    <t>0899 Y</t>
+  </si>
+  <si>
+    <t>CANALES 49-2</t>
+  </si>
+  <si>
+    <t>0911 Y</t>
+  </si>
+  <si>
+    <t>0922 Y</t>
   </si>
 </sst>
 </file>
@@ -3016,10 +3025,10 @@
   <dimension ref="A1:X291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="H7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3175,7 +3184,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4" s="39"/>
       <c r="E4" s="40"/>
@@ -3186,7 +3195,7 @@
         <v>44564</v>
       </c>
       <c r="H4" s="43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I4" s="44">
         <v>21980</v>
@@ -3205,7 +3214,7 @@
         <v>824250</v>
       </c>
       <c r="O4" s="396" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P4" s="398">
         <v>44578</v>
@@ -3235,7 +3244,7 @@
         <v>33</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D5" s="60"/>
       <c r="E5" s="40"/>
@@ -3246,7 +3255,7 @@
         <v>44564</v>
       </c>
       <c r="H5" s="63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I5" s="64">
         <v>4770</v>
@@ -3265,7 +3274,7 @@
         <v>176375</v>
       </c>
       <c r="O5" s="399" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P5" s="400">
         <v>44578</v>
@@ -3294,7 +3303,9 @@
       <c r="B6" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="59"/>
+      <c r="C6" s="59" t="s">
+        <v>92</v>
+      </c>
       <c r="D6" s="60"/>
       <c r="E6" s="40"/>
       <c r="F6" s="61">
@@ -3304,7 +3315,7 @@
         <v>44566</v>
       </c>
       <c r="H6" s="403" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I6" s="64">
         <f>21870-109.35</f>
@@ -3324,7 +3335,7 @@
         <v>816024.375</v>
       </c>
       <c r="O6" s="399" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P6" s="400">
         <v>44580</v>
@@ -3351,9 +3362,11 @@
         <v>22</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="59"/>
+        <v>93</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>92</v>
+      </c>
       <c r="D7" s="60"/>
       <c r="E7" s="40"/>
       <c r="F7" s="61">
@@ -3363,7 +3376,7 @@
         <v>44566</v>
       </c>
       <c r="H7" s="63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I7" s="64">
         <v>5415</v>
@@ -3382,7 +3395,7 @@
         <v>203062.5</v>
       </c>
       <c r="O7" s="399" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P7" s="400">
         <v>44580</v>
@@ -3406,12 +3419,14 @@
     </row>
     <row r="8" spans="1:24" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="58" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="59"/>
+      <c r="C8" s="59" t="s">
+        <v>94</v>
+      </c>
       <c r="D8" s="60"/>
       <c r="E8" s="40"/>
       <c r="F8" s="61">
@@ -3421,7 +3436,7 @@
         <v>44568</v>
       </c>
       <c r="H8" s="63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I8" s="64">
         <f>20760-103.8</f>
@@ -3441,7 +3456,7 @@
         <v>774607.5</v>
       </c>
       <c r="O8" s="90" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P8" s="91">
         <v>44582</v>
@@ -3465,12 +3480,14 @@
     </row>
     <row r="9" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="59"/>
+      <c r="C9" s="59" t="s">
+        <v>94</v>
+      </c>
       <c r="D9" s="60"/>
       <c r="E9" s="40"/>
       <c r="F9" s="61">
@@ -3480,7 +3497,7 @@
         <v>44568</v>
       </c>
       <c r="H9" s="63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I9" s="64">
         <v>5595</v>
@@ -3499,7 +3516,7 @@
         <v>209812.5</v>
       </c>
       <c r="O9" s="90" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P9" s="91">
         <v>44582</v>
@@ -3523,12 +3540,14 @@
     </row>
     <row r="10" spans="1:24" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="71" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="58" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="59"/>
+        <v>41</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>95</v>
+      </c>
       <c r="D10" s="72"/>
       <c r="E10" s="40"/>
       <c r="F10" s="61">
@@ -3538,7 +3557,7 @@
         <v>44570</v>
       </c>
       <c r="H10" s="63" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I10" s="64">
         <f>22600-113</f>
@@ -3558,7 +3577,7 @@
         <v>843262.5</v>
       </c>
       <c r="O10" s="401" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P10" s="402">
         <v>44585</v>
@@ -3580,14 +3599,16 @@
         <v>4176</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="71" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="59"/>
+        <v>38</v>
+      </c>
+      <c r="C11" s="59" t="s">
+        <v>95</v>
+      </c>
       <c r="D11" s="60"/>
       <c r="E11" s="40"/>
       <c r="F11" s="61">
@@ -3597,7 +3618,7 @@
         <v>44570</v>
       </c>
       <c r="H11" s="63" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I11" s="64">
         <v>5535</v>
@@ -3616,7 +3637,7 @@
         <v>207562.5</v>
       </c>
       <c r="O11" s="401" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P11" s="402">
         <v>44585</v>
@@ -3643,7 +3664,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="60"/>
@@ -3655,7 +3676,7 @@
         <v>44574</v>
       </c>
       <c r="H12" s="63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I12" s="64">
         <v>24170</v>
@@ -3674,7 +3695,7 @@
         <v>894290</v>
       </c>
       <c r="O12" s="401" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P12" s="402">
         <v>44587</v>
@@ -3698,7 +3719,7 @@
     </row>
     <row r="13" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="71" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="58" t="s">
         <v>33</v>
@@ -3713,7 +3734,7 @@
         <v>44574</v>
       </c>
       <c r="H13" s="63" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" s="64">
         <v>5995</v>
@@ -3732,7 +3753,7 @@
         <v>221815</v>
       </c>
       <c r="O13" s="401" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P13" s="402">
         <v>44587</v>
@@ -3756,10 +3777,10 @@
     </row>
     <row r="14" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="71" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="58" t="s">
         <v>49</v>
-      </c>
-      <c r="B14" s="58" t="s">
-        <v>50</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="60"/>
@@ -3771,7 +3792,7 @@
         <v>44575</v>
       </c>
       <c r="H14" s="63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I14" s="64">
         <v>20605</v>
@@ -3790,7 +3811,7 @@
         <v>762385</v>
       </c>
       <c r="O14" s="401" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P14" s="402">
         <v>44589</v>
@@ -3814,10 +3835,10 @@
     </row>
     <row r="15" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="58" t="s">
         <v>38</v>
-      </c>
-      <c r="B15" s="58" t="s">
-        <v>39</v>
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="60"/>
@@ -3829,7 +3850,7 @@
         <v>44575</v>
       </c>
       <c r="H15" s="63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I15" s="64">
         <v>5595</v>
@@ -3848,7 +3869,7 @@
         <v>207015</v>
       </c>
       <c r="O15" s="401" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P15" s="402">
         <v>44589</v>
@@ -3872,7 +3893,7 @@
     </row>
     <row r="16" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="58" t="s">
         <v>32</v>
@@ -3887,7 +3908,7 @@
         <v>44577</v>
       </c>
       <c r="H16" s="63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I16" s="64">
         <v>22370</v>
@@ -3906,7 +3927,7 @@
         <v>816505</v>
       </c>
       <c r="O16" s="401" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P16" s="402">
         <v>44592</v>
@@ -3930,10 +3951,10 @@
     </row>
     <row r="17" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="75" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="58" t="s">
         <v>38</v>
-      </c>
-      <c r="B17" s="58" t="s">
-        <v>39</v>
       </c>
       <c r="C17" s="59"/>
       <c r="D17" s="60"/>
@@ -3945,7 +3966,7 @@
         <v>44577</v>
       </c>
       <c r="H17" s="63" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I17" s="64">
         <v>5755</v>
@@ -3964,7 +3985,7 @@
         <v>210057.5</v>
       </c>
       <c r="O17" s="401" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P17" s="402">
         <v>44592</v>
@@ -3988,10 +4009,10 @@
     </row>
     <row r="18" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="78" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="60"/>
@@ -4003,7 +4024,7 @@
         <v>44578</v>
       </c>
       <c r="H18" s="63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I18" s="64">
         <v>21630</v>
@@ -4022,7 +4043,7 @@
         <v>789495</v>
       </c>
       <c r="O18" s="401" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P18" s="402">
         <v>44592</v>
@@ -4046,10 +4067,10 @@
     </row>
     <row r="19" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="78" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="58" t="s">
         <v>53</v>
-      </c>
-      <c r="B19" s="58" t="s">
-        <v>54</v>
       </c>
       <c r="C19" s="59"/>
       <c r="D19" s="60"/>
@@ -4061,7 +4082,7 @@
         <v>44581</v>
       </c>
       <c r="H19" s="63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I19" s="64">
         <v>21970</v>
@@ -4100,10 +4121,10 @@
     </row>
     <row r="20" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="80" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="58" t="s">
         <v>38</v>
-      </c>
-      <c r="B20" s="58" t="s">
-        <v>39</v>
       </c>
       <c r="C20" s="59"/>
       <c r="D20" s="60"/>
@@ -4115,7 +4136,7 @@
         <v>44581</v>
       </c>
       <c r="H20" s="63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I20" s="64">
         <v>5745</v>
@@ -4154,10 +4175,10 @@
     </row>
     <row r="21" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="58" t="s">
         <v>72</v>
-      </c>
-      <c r="B21" s="58" t="s">
-        <v>73</v>
       </c>
       <c r="C21" s="59"/>
       <c r="D21" s="60"/>
@@ -4169,7 +4190,7 @@
         <v>44582</v>
       </c>
       <c r="H21" s="63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I21" s="64">
         <v>22350</v>
@@ -4211,7 +4232,7 @@
         <v>23</v>
       </c>
       <c r="B22" s="58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="59"/>
       <c r="D22" s="60"/>
@@ -4223,7 +4244,7 @@
         <v>44582</v>
       </c>
       <c r="H22" s="63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I22" s="64">
         <v>5420</v>
@@ -4262,10 +4283,10 @@
     </row>
     <row r="23" spans="1:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="82" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="59"/>
       <c r="D23" s="60"/>
@@ -4366,10 +4387,10 @@
     </row>
     <row r="25" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="71" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="58" t="s">
         <v>76</v>
-      </c>
-      <c r="B25" s="58" t="s">
-        <v>77</v>
       </c>
       <c r="C25" s="87"/>
       <c r="D25" s="88"/>
@@ -4418,10 +4439,10 @@
     </row>
     <row r="26" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="82" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B26" s="58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="87"/>
       <c r="D26" s="88"/>
@@ -4470,10 +4491,10 @@
     </row>
     <row r="27" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="82" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C27" s="59"/>
       <c r="D27" s="60"/>
@@ -4522,7 +4543,7 @@
     </row>
     <row r="28" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="82" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="58" t="s">
         <v>33</v>
@@ -4574,10 +4595,10 @@
     </row>
     <row r="29" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" s="94" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C29" s="59"/>
       <c r="D29" s="60"/>
@@ -4622,7 +4643,7 @@
     </row>
     <row r="30" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30" s="94" t="s">
         <v>33</v>
@@ -5503,13 +5524,13 @@
     </row>
     <row r="55" spans="1:24" s="162" customFormat="1" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B55" s="149" t="s">
         <v>24</v>
       </c>
       <c r="C55" s="150" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D55" s="151"/>
       <c r="E55" s="40">
@@ -5542,7 +5563,7 @@
         <v>167804</v>
       </c>
       <c r="O55" s="90" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P55" s="163">
         <v>44572</v>
@@ -5768,13 +5789,13 @@
     </row>
     <row r="62" spans="1:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="177" t="s">
+        <v>44</v>
+      </c>
+      <c r="B62" s="395" t="s">
         <v>45</v>
       </c>
-      <c r="B62" s="395" t="s">
+      <c r="C62" s="178" t="s">
         <v>46</v>
-      </c>
-      <c r="C62" s="178" t="s">
-        <v>47</v>
       </c>
       <c r="D62" s="179"/>
       <c r="E62" s="40">
@@ -5788,7 +5809,7 @@
         <v>44565</v>
       </c>
       <c r="H62" s="154" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I62" s="152">
         <v>410</v>
@@ -5807,7 +5828,7 @@
         <v>26650</v>
       </c>
       <c r="O62" s="167" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P62" s="163">
         <v>44572</v>
@@ -5821,13 +5842,13 @@
     </row>
     <row r="63" spans="1:24" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A63" s="397" t="s">
+        <v>54</v>
+      </c>
+      <c r="B63" s="386" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="386" t="s">
+      <c r="C63" s="182" t="s">
         <v>56</v>
-      </c>
-      <c r="C63" s="182" t="s">
-        <v>57</v>
       </c>
       <c r="D63" s="384"/>
       <c r="E63" s="40"/>
@@ -5865,7 +5886,7 @@
     </row>
     <row r="64" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A64" s="180" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B64" s="181"/>
       <c r="C64" s="186"/>
@@ -5900,7 +5921,7 @@
     </row>
     <row r="65" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A65" s="180" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B65" s="181"/>
       <c r="C65" s="186"/>
@@ -5935,13 +5956,13 @@
     </row>
     <row r="66" spans="1:22" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="180" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" s="181" t="s">
         <v>45</v>
       </c>
-      <c r="B66" s="181" t="s">
-        <v>46</v>
-      </c>
       <c r="C66" s="186" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D66" s="174"/>
       <c r="E66" s="60">
@@ -5955,7 +5976,7 @@
         <v>44579</v>
       </c>
       <c r="H66" s="154" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I66" s="152">
         <v>300</v>
@@ -5974,7 +5995,7 @@
         <v>19500</v>
       </c>
       <c r="O66" s="167" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P66" s="184">
         <v>44579</v>
@@ -5988,7 +6009,7 @@
     </row>
     <row r="67" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A67" s="185" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B67" s="181"/>
       <c r="C67" s="174"/>
@@ -6023,13 +6044,13 @@
     </row>
     <row r="68" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="180" t="s">
+        <v>44</v>
+      </c>
+      <c r="B68" s="181" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="181" t="s">
-        <v>46</v>
-      </c>
       <c r="C68" s="186" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D68" s="174"/>
       <c r="E68" s="60">
@@ -6043,7 +6064,7 @@
         <v>44582</v>
       </c>
       <c r="H68" s="154" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I68" s="152">
         <v>430</v>
@@ -6062,7 +6083,7 @@
         <v>27950</v>
       </c>
       <c r="O68" s="167" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P68" s="184">
         <v>44585</v>

</xml_diff>

<commit_message>
CIERRE  11 FEB 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/ENTRADAS OBRADOR ENERO 2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/ENTRADAS OBRADOR ENERO 2022.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="106">
   <si>
     <t>FECHA DE PAGO</t>
   </si>
@@ -336,6 +336,12 @@
   </si>
   <si>
     <t>0060 Z</t>
+  </si>
+  <si>
+    <t>0073 Z</t>
+  </si>
+  <si>
+    <t>0085 Z</t>
   </si>
 </sst>
 </file>
@@ -2662,6 +2668,78 @@
     <xf numFmtId="4" fontId="2" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2689,82 +2767,10 @@
     <xf numFmtId="4" fontId="32" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3058,10 +3064,10 @@
   <dimension ref="A1:X291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="H55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3090,18 +3096,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="407" t="s">
+      <c r="A1" s="431" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="407"/>
-      <c r="C1" s="407"/>
-      <c r="D1" s="407"/>
-      <c r="E1" s="407"/>
-      <c r="F1" s="407"/>
-      <c r="G1" s="407"/>
-      <c r="H1" s="407"/>
-      <c r="I1" s="407"/>
-      <c r="J1" s="407"/>
+      <c r="B1" s="431"/>
+      <c r="C1" s="431"/>
+      <c r="D1" s="431"/>
+      <c r="E1" s="431"/>
+      <c r="F1" s="431"/>
+      <c r="G1" s="431"/>
+      <c r="H1" s="431"/>
+      <c r="I1" s="431"/>
+      <c r="J1" s="431"/>
       <c r="K1" s="378"/>
       <c r="L1" s="378"/>
       <c r="M1" s="378"/>
@@ -3115,22 +3121,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="408" t="s">
+      <c r="W1" s="432" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="409"/>
+      <c r="X1" s="433"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="407"/>
-      <c r="B2" s="407"/>
-      <c r="C2" s="407"/>
-      <c r="D2" s="407"/>
-      <c r="E2" s="407"/>
-      <c r="F2" s="407"/>
-      <c r="G2" s="407"/>
-      <c r="H2" s="407"/>
-      <c r="I2" s="407"/>
-      <c r="J2" s="407"/>
+      <c r="A2" s="431"/>
+      <c r="B2" s="431"/>
+      <c r="C2" s="431"/>
+      <c r="D2" s="431"/>
+      <c r="E2" s="431"/>
+      <c r="F2" s="431"/>
+      <c r="G2" s="431"/>
+      <c r="H2" s="431"/>
+      <c r="I2" s="431"/>
+      <c r="J2" s="431"/>
       <c r="K2" s="380"/>
       <c r="L2" s="380"/>
       <c r="M2" s="380"/>
@@ -3184,10 +3190,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="410" t="s">
+      <c r="O3" s="434" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="411"/>
+      <c r="P3" s="435"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -4555,7 +4561,9 @@
       <c r="B27" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="59"/>
+      <c r="C27" s="59" t="s">
+        <v>104</v>
+      </c>
       <c r="D27" s="60"/>
       <c r="E27" s="40"/>
       <c r="F27" s="61">
@@ -4607,7 +4615,9 @@
       <c r="B28" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="59"/>
+      <c r="C28" s="59" t="s">
+        <v>104</v>
+      </c>
       <c r="D28" s="60"/>
       <c r="E28" s="40"/>
       <c r="F28" s="61">
@@ -4659,7 +4669,9 @@
       <c r="B29" s="93" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="59"/>
+      <c r="C29" s="59" t="s">
+        <v>105</v>
+      </c>
       <c r="D29" s="60"/>
       <c r="E29" s="40"/>
       <c r="F29" s="61">
@@ -4707,7 +4719,9 @@
       <c r="B30" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="59"/>
+      <c r="C30" s="59" t="s">
+        <v>105</v>
+      </c>
       <c r="D30" s="60"/>
       <c r="E30" s="40"/>
       <c r="F30" s="61">
@@ -5672,11 +5686,11 @@
       <c r="X56"/>
     </row>
     <row r="57" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="412"/>
+      <c r="A57" s="436"/>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="414"/>
+      <c r="C57" s="438"/>
       <c r="D57" s="167"/>
       <c r="E57" s="40">
         <f t="shared" si="2"/>
@@ -5684,7 +5698,7 @@
       </c>
       <c r="F57" s="151"/>
       <c r="G57" s="152"/>
-      <c r="H57" s="416"/>
+      <c r="H57" s="424"/>
       <c r="I57" s="151"/>
       <c r="J57" s="45">
         <f t="shared" si="0"/>
@@ -5697,8 +5711,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O57" s="418"/>
-      <c r="P57" s="420"/>
+      <c r="O57" s="409"/>
+      <c r="P57" s="426"/>
       <c r="Q57" s="166"/>
       <c r="R57" s="129"/>
       <c r="S57" s="92"/>
@@ -5707,11 +5721,11 @@
       <c r="V57" s="54"/>
     </row>
     <row r="58" spans="1:24" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="413"/>
+      <c r="A58" s="437"/>
       <c r="B58" s="148" t="s">
         <v>25</v>
       </c>
-      <c r="C58" s="415"/>
+      <c r="C58" s="439"/>
       <c r="D58" s="167"/>
       <c r="E58" s="40">
         <f t="shared" si="2"/>
@@ -5719,7 +5733,7 @@
       </c>
       <c r="F58" s="151"/>
       <c r="G58" s="152"/>
-      <c r="H58" s="417"/>
+      <c r="H58" s="425"/>
       <c r="I58" s="151"/>
       <c r="J58" s="45">
         <f t="shared" si="0"/>
@@ -5732,8 +5746,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O58" s="419"/>
-      <c r="P58" s="421"/>
+      <c r="O58" s="440"/>
+      <c r="P58" s="441"/>
       <c r="Q58" s="166"/>
       <c r="R58" s="129"/>
       <c r="S58" s="92"/>
@@ -5742,11 +5756,11 @@
       <c r="V58" s="54"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="425"/>
+      <c r="A59" s="420"/>
       <c r="B59" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="427"/>
+      <c r="C59" s="422"/>
       <c r="D59" s="165"/>
       <c r="E59" s="40">
         <f t="shared" si="2"/>
@@ -5754,7 +5768,7 @@
       </c>
       <c r="F59" s="151"/>
       <c r="G59" s="152"/>
-      <c r="H59" s="416"/>
+      <c r="H59" s="424"/>
       <c r="I59" s="151"/>
       <c r="J59" s="45">
         <f t="shared" si="0"/>
@@ -5779,11 +5793,11 @@
       <c r="X59"/>
     </row>
     <row r="60" spans="1:24" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="426"/>
+      <c r="A60" s="421"/>
       <c r="B60" s="148" t="s">
         <v>25</v>
       </c>
-      <c r="C60" s="428"/>
+      <c r="C60" s="423"/>
       <c r="D60" s="170"/>
       <c r="E60" s="40">
         <f t="shared" si="2"/>
@@ -5791,7 +5805,7 @@
       </c>
       <c r="F60" s="151"/>
       <c r="G60" s="152"/>
-      <c r="H60" s="417"/>
+      <c r="H60" s="425"/>
       <c r="I60" s="151"/>
       <c r="J60" s="45">
         <f t="shared" si="0"/>
@@ -5969,8 +5983,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O64" s="418"/>
-      <c r="P64" s="420"/>
+      <c r="O64" s="409"/>
+      <c r="P64" s="426"/>
       <c r="Q64" s="166"/>
       <c r="R64" s="129"/>
       <c r="S64" s="182"/>
@@ -6004,8 +6018,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O65" s="429"/>
-      <c r="P65" s="430"/>
+      <c r="O65" s="410"/>
+      <c r="P65" s="427"/>
       <c r="Q65" s="166"/>
       <c r="R65" s="129"/>
       <c r="S65" s="182"/>
@@ -6277,8 +6291,8 @@
         <f>K72*I72</f>
         <v>0</v>
       </c>
-      <c r="O72" s="431"/>
-      <c r="P72" s="422"/>
+      <c r="O72" s="428"/>
+      <c r="P72" s="417"/>
       <c r="Q72" s="169"/>
       <c r="R72" s="129"/>
       <c r="S72" s="182"/>
@@ -6310,8 +6324,8 @@
         <f>K73*I73</f>
         <v>0</v>
       </c>
-      <c r="O73" s="432"/>
-      <c r="P73" s="423"/>
+      <c r="O73" s="429"/>
+      <c r="P73" s="418"/>
       <c r="Q73" s="169"/>
       <c r="R73" s="129"/>
       <c r="S73" s="182"/>
@@ -6343,8 +6357,8 @@
         <f>K74*I74</f>
         <v>0</v>
       </c>
-      <c r="O74" s="432"/>
-      <c r="P74" s="423"/>
+      <c r="O74" s="429"/>
+      <c r="P74" s="418"/>
       <c r="Q74" s="169"/>
       <c r="R74" s="129"/>
       <c r="S74" s="182"/>
@@ -6376,8 +6390,8 @@
         <f>K75*I75</f>
         <v>0</v>
       </c>
-      <c r="O75" s="433"/>
-      <c r="P75" s="424"/>
+      <c r="O75" s="430"/>
+      <c r="P75" s="419"/>
       <c r="Q75" s="169"/>
       <c r="R75" s="129"/>
       <c r="S75" s="182"/>
@@ -6475,8 +6489,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O78" s="418"/>
-      <c r="P78" s="440"/>
+      <c r="O78" s="409"/>
+      <c r="P78" s="415"/>
       <c r="Q78" s="166"/>
       <c r="R78" s="129"/>
       <c r="S78" s="182"/>
@@ -6508,8 +6522,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="429"/>
-      <c r="P79" s="441"/>
+      <c r="O79" s="410"/>
+      <c r="P79" s="416"/>
       <c r="Q79" s="166"/>
       <c r="R79" s="129"/>
       <c r="S79" s="182"/>
@@ -6541,8 +6555,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="418"/>
-      <c r="P80" s="440"/>
+      <c r="O80" s="409"/>
+      <c r="P80" s="415"/>
       <c r="Q80" s="166"/>
       <c r="R80" s="158"/>
       <c r="S80" s="182"/>
@@ -6574,8 +6588,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="429"/>
-      <c r="P81" s="441"/>
+      <c r="O81" s="410"/>
+      <c r="P81" s="416"/>
       <c r="Q81" s="166"/>
       <c r="R81" s="158"/>
       <c r="S81" s="182"/>
@@ -6733,8 +6747,8 @@
         <v>0</v>
       </c>
       <c r="K86" s="100"/>
-      <c r="L86" s="434"/>
-      <c r="M86" s="435"/>
+      <c r="L86" s="407"/>
+      <c r="M86" s="408"/>
       <c r="N86" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -6766,8 +6780,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="434"/>
-      <c r="M87" s="435"/>
+      <c r="L87" s="407"/>
+      <c r="M87" s="408"/>
       <c r="N87" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -6970,8 +6984,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O93" s="418"/>
-      <c r="P93" s="436"/>
+      <c r="O93" s="409"/>
+      <c r="P93" s="411"/>
       <c r="Q93" s="166"/>
       <c r="R93" s="129"/>
       <c r="S93" s="182"/>
@@ -7003,8 +7017,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="429"/>
-      <c r="P94" s="437"/>
+      <c r="O94" s="410"/>
+      <c r="P94" s="412"/>
       <c r="Q94" s="166"/>
       <c r="R94" s="129"/>
       <c r="S94" s="182"/>
@@ -12396,11 +12410,11 @@
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F258" s="438" t="s">
+      <c r="F258" s="413" t="s">
         <v>27</v>
       </c>
-      <c r="G258" s="438"/>
-      <c r="H258" s="439"/>
+      <c r="G258" s="413"/>
+      <c r="H258" s="414"/>
       <c r="I258" s="320">
         <f>SUM(I4:I257)</f>
         <v>420295.66</v>
@@ -12974,6 +12988,21 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="O57:O58"/>
+    <mergeCell ref="P57:P58"/>
+    <mergeCell ref="P72:P75"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="O64:O65"/>
+    <mergeCell ref="P64:P65"/>
+    <mergeCell ref="O72:O75"/>
     <mergeCell ref="L86:M87"/>
     <mergeCell ref="O93:O94"/>
     <mergeCell ref="P93:P94"/>
@@ -12982,21 +13011,6 @@
     <mergeCell ref="P78:P79"/>
     <mergeCell ref="O80:O81"/>
     <mergeCell ref="P80:P81"/>
-    <mergeCell ref="P72:P75"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="O64:O65"/>
-    <mergeCell ref="P64:P65"/>
-    <mergeCell ref="O72:O75"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="O57:O58"/>
-    <mergeCell ref="P57:P58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>